<commit_message>
Ocultação dos nomes das empresas
</commit_message>
<xml_diff>
--- a/Estudo sobre Feedback do Usuário na Engenharia de Software (respostas) - Copia.xlsx
+++ b/Estudo sobre Feedback do Usuário na Engenharia de Software (respostas) - Copia.xlsx
@@ -1,27 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Meu Drive\1 - UFES\UFES - 2024_2025\2024 -2 - 2025-1\Survey\Escrita - materiais\Artigo\repositorio anonimizado\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Meu Drive\1 - UFES\UFES - 2024_2025\2024 -2 - 2025-1\Survey\Artigo\Dados_Survey_Estudo_Sobre_Feedback\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{671ECAFB-D4B6-4852-840F-958D2C1C1D7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB109F94-A9F9-4188-83F3-71F01FE4F6D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1080" yWindow="1080" windowWidth="17910" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Respostas ao formulário 1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="695" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="705" uniqueCount="283">
   <si>
     <t>Carimbo de data/hora</t>
   </si>
@@ -306,9 +305,6 @@
 Use o espaço a seguir para compartilhar informações que você julgue relevantes sobre feedback de usuário (por exemplo, aspectos que não foram abordados no questionário e que você ache pertinente registrar, comentários gerais sobre o tema considerando sua experiência na área). Sinta-se à vontade também para indicar se você teve alguma dificuldade para responder o questionário, se você tem alguma crítica ou sugestão de melhoria.</t>
   </si>
   <si>
-    <t>E&amp;L Produções de Software</t>
-  </si>
-  <si>
     <t>ES - Espírito Santo</t>
   </si>
   <si>
@@ -369,9 +365,6 @@
     <t xml:space="preserve">Qualquer organização que coleta feedback precisa estar disposta a valorizar a opinião das pessoas pesquisadas.  </t>
   </si>
   <si>
-    <t>FURB - LDTT</t>
-  </si>
-  <si>
     <t>SC - Santa Catarina</t>
   </si>
   <si>
@@ -417,9 +410,6 @@
     <t>Alguns tópicos não são comuns para o profissional de TI. Mas o Feedback é algo rotineiro na organização. O processo poderia ser melhor estruturado</t>
   </si>
   <si>
-    <t>Grupo Pão de Açúcar</t>
-  </si>
-  <si>
     <t>SP - São Paulo</t>
   </si>
   <si>
@@ -465,9 +455,6 @@
     <t>Acredito que poderíamos incluir essa coleta de feedbacks na sprint de um scrum?</t>
   </si>
   <si>
-    <t>IDEMA - Natal RN</t>
-  </si>
-  <si>
     <t>RN - Rio Grande do Norte</t>
   </si>
   <si>
@@ -504,9 +491,6 @@
     <t>Parabéns pelo trabalho</t>
   </si>
   <si>
-    <t>IDERA TECNOLOGIA</t>
-  </si>
-  <si>
     <t>1 - 9 funcionários</t>
   </si>
   <si>
@@ -531,9 +515,6 @@
     <t>Não tenho o que acrescentar.</t>
   </si>
   <si>
-    <t>Imagem Geosistemas</t>
-  </si>
-  <si>
     <t>Prestadora de Serviços de software de Geoprocessamento</t>
   </si>
   <si>
@@ -561,9 +542,6 @@
     <t>Na empresa onde trabalho o Feedback dos clientes faz parte de um indicador estratégico, então é tratado com muito rigor e a empresa investe em ações corretivas para tratar os problemas identificados.</t>
   </si>
   <si>
-    <t>Imobiliaria Betha Espaço</t>
-  </si>
-  <si>
     <t>50 a 99 funcionários</t>
   </si>
   <si>
@@ -594,9 +572,6 @@
     <t>A maior dificuldade encontrada no levantamento de requisitos e a obtenção de feedback, acontece quando os usuários não tem domínio completo do contexto do processo que precisa ser executado. Dessa forma o processo precisa ser reparado ou alterado com frequência o que gera o loop no desenvolvimento e solicitação de testes e feedback.</t>
   </si>
   <si>
-    <t xml:space="preserve">Instituto Federal de Educação, Ciência e Tecnologia do Amazonas </t>
-  </si>
-  <si>
     <t>AM - Amazonas</t>
   </si>
   <si>
@@ -621,9 +596,6 @@
     <t xml:space="preserve">Ao participar desta pesquisa percebi que coletar e analisar feedback dos utilizadores pode ser muito útil para desenvolvimento de melhores produtos. Pretendo dar mais atenção a essa área daqui pra frente. </t>
   </si>
   <si>
-    <t>Laboratório de Pesquisa Operacional UFPA</t>
-  </si>
-  <si>
     <t>PA - Pará</t>
   </si>
   <si>
@@ -657,9 +629,6 @@
     <t xml:space="preserve">Acho que dados qualitativos abordados nesse questionário, são bem pertinentes. </t>
   </si>
   <si>
-    <t>Leds/ifes</t>
-  </si>
-  <si>
     <t>Uso de métodos ágeis (por exemplo, Scrum, XP), Uso de métodos de Engenharia de Software Contínua (por exemplo, DevOps, Lean Thinking), Desenvolvimento híbrido, que combina práticas de métodos sequenciais e orientados a planejamento com práticas ágeis  ou de Engenharia de Software Contínua</t>
   </si>
   <si>
@@ -678,9 +647,6 @@
     <t>Acreditamos que, além dos benefícios operacionais e financeiros, os projetos também podem impactar aspectos sociais e humanos dentro da organização, como questões de saúde e bem-estar dos colaboradores. Por exemplo, implementamos um projeto onde o trabalho excessivamente repetitivo estava causando LER (Lesão por Esforço Repetitivo) nos funcionários. Além disso, havia dificuldades na divulgação dos resultados desse trabalho. Com a implantação do projeto, o trabalho repetitivo foi eliminado, reduzindo o risco de lesões, e os resultados passaram a ser divulgados de forma transparente. Coletar esse tipo de feedback é essencial para avaliar melhorias organizacionais que vão além da eficiência operacional.</t>
   </si>
   <si>
-    <t>Mosyle</t>
-  </si>
-  <si>
     <t>Organização em que um único produto de software representa o negócio (por exemplo, PicPay, Airbnb, Uber)</t>
   </si>
   <si>
@@ -705,9 +671,6 @@
     <t>Os feedbacks geralmente são coletados usando as ferramentas internas da empresa, mas esses feedbacks geralmente ocorrem quem algo dá errado, então são abertos alguns chamados para o suporte técnico, que é a área que coleta o feedback com o cliente geralmente via chat ou tele atendimento.</t>
   </si>
   <si>
-    <t>Projeto CIN / Motorola</t>
-  </si>
-  <si>
     <t>PE - Pernambuco</t>
   </si>
   <si>
@@ -738,9 +701,6 @@
     <t>N/A</t>
   </si>
   <si>
-    <t>Projetos de P&amp;D desenvolvidos no Laboratório da UFMA</t>
-  </si>
-  <si>
     <t>MA - Maranhão</t>
   </si>
   <si>
@@ -762,9 +722,6 @@
     <t>Nada a declarar.</t>
   </si>
   <si>
-    <t>Projetos de Pesquisa Universidade de Brasília x Governo Federal (UnB)</t>
-  </si>
-  <si>
     <t>DF - Distrito Federal</t>
   </si>
   <si>
@@ -789,9 +746,6 @@
     <t xml:space="preserve">O feedback de usuário dependendo da aplicação é mais complexo. Em alguns cenários em que os usuários não possuem um nível de escolaridade por exemplo, é extremamente difícil coletas o feedback deles. Já trabalhamos em aplicações envolvendo egressos brasileiros do sistema prisional que tivemos que retirar a opção de avaliação por parte dos usuários. Entendo que é importante, mas infelizmente em populações sensíveis não é possível realizar e coletar o feedback do usuário usando técnicas disponíveis e comumente usadas. </t>
   </si>
   <si>
-    <t>SENAI RR</t>
-  </si>
-  <si>
     <t>RR - Roraima</t>
   </si>
   <si>
@@ -813,9 +767,6 @@
     <t>Além da coleta e análise, é fundamental garantir que as sugestões sejam realmente consideradas e resultem em ações concretas. Um desafio comum é engajar os usuários para fornecerem feedback detalhado e relevante.</t>
   </si>
   <si>
-    <t>Siemens Healthineers</t>
-  </si>
-  <si>
     <t>Uso de métodos ágeis (por exemplo, Scrum, XP), Uso de métodos de Engenharia de Software Contínua (por exemplo, DevOps, Lean Thinking)</t>
   </si>
   <si>
@@ -834,9 +785,6 @@
     <t>feedbacks do usuário são a capacidade de detecção da direção para o crescimento</t>
   </si>
   <si>
-    <t xml:space="preserve">Stefanini </t>
-  </si>
-  <si>
     <t>RJ - Rio de Janeiro</t>
   </si>
   <si>
@@ -855,9 +803,6 @@
     <t>Nada a declarar</t>
   </si>
   <si>
-    <t>TJRO</t>
-  </si>
-  <si>
     <t>RO - Rondônia</t>
   </si>
   <si>
@@ -879,9 +824,6 @@
     <t>Os feedback dos usuários devem ser colhidos com frequência, especialmente após atualizações dos sistemas. Em uma empresa pequena é possível fazer esse acompanhamento no dia a dia com os usuários e atender imediatamente os feedbacks, implementado-os no sistema. Quanto maior a organização</t>
   </si>
   <si>
-    <t>TRT</t>
-  </si>
-  <si>
     <t>Líder Técnico</t>
   </si>
   <si>
@@ -894,9 +836,6 @@
     <t>Avaliação geral da TI do órgão</t>
   </si>
   <si>
-    <t>Vallourec</t>
-  </si>
-  <si>
     <t>MG - Minas Gerais</t>
   </si>
   <si>
@@ -913,9 +852,6 @@
   </si>
   <si>
     <t>Achei válido a pesquisa e sinto honrado em participar.  Não obtive dificuldade em responder . Minha dica é tanto como desenvolvedor de sistemas e também como usuário, a ferramenta de feedback é importantíssima, um usuário que recebe o retorno de um feedback que foi positivo ou negativo pode ter certeza que sente valorizado e tem muito mais a agregar ao produto.</t>
-  </si>
-  <si>
-    <t>Xertica</t>
   </si>
   <si>
     <t>Startup</t>
@@ -1062,6 +998,99 @@
   <si>
     <t>...........</t>
   </si>
+  <si>
+    <t>Org 1</t>
+  </si>
+  <si>
+    <t>Org 2</t>
+  </si>
+  <si>
+    <t>Org 8</t>
+  </si>
+  <si>
+    <t>Org 6</t>
+  </si>
+  <si>
+    <t>Org 3</t>
+  </si>
+  <si>
+    <t>Org 4</t>
+  </si>
+  <si>
+    <t>Org 5</t>
+  </si>
+  <si>
+    <t>Org 7</t>
+  </si>
+  <si>
+    <t>Org 9</t>
+  </si>
+  <si>
+    <t>Org 10</t>
+  </si>
+  <si>
+    <t>Org 11</t>
+  </si>
+  <si>
+    <t>Org 12</t>
+  </si>
+  <si>
+    <t>Org 13</t>
+  </si>
+  <si>
+    <t>Org 14</t>
+  </si>
+  <si>
+    <t>Org 15</t>
+  </si>
+  <si>
+    <t>Org 16</t>
+  </si>
+  <si>
+    <t>Org 17</t>
+  </si>
+  <si>
+    <t>Org 18</t>
+  </si>
+  <si>
+    <t>Org 19</t>
+  </si>
+  <si>
+    <t>Org 20</t>
+  </si>
+  <si>
+    <t>Org 21</t>
+  </si>
+  <si>
+    <t>Org 22</t>
+  </si>
+  <si>
+    <t>Org 23</t>
+  </si>
+  <si>
+    <t>Org 24</t>
+  </si>
+  <si>
+    <t>Org 25</t>
+  </si>
+  <si>
+    <t>Org 26</t>
+  </si>
+  <si>
+    <t>Org 27</t>
+  </si>
+  <si>
+    <t>Org 28</t>
+  </si>
+  <si>
+    <t>Org 29</t>
+  </si>
+  <si>
+    <t>Org 30</t>
+  </si>
+  <si>
+    <t>Org 31</t>
+  </si>
 </sst>
 </file>
 
@@ -1070,7 +1099,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yyyy\ h:mm:ss"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1093,6 +1122,11 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1616,21 +1650,21 @@
   <dimension ref="A1:W32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
+      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.42578125" customWidth="1"/>
+    <col min="1" max="1" width="24.44140625" customWidth="1"/>
     <col min="2" max="2" width="53" customWidth="1"/>
-    <col min="3" max="3" width="37.140625" customWidth="1"/>
-    <col min="4" max="4" width="32.5703125" customWidth="1"/>
-    <col min="5" max="23" width="37.5703125" customWidth="1"/>
-    <col min="24" max="29" width="18.85546875" customWidth="1"/>
+    <col min="3" max="3" width="37.109375" customWidth="1"/>
+    <col min="4" max="4" width="32.5546875" customWidth="1"/>
+    <col min="5" max="23" width="37.5546875" customWidth="1"/>
+    <col min="24" max="29" width="18.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:23" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1701,2185 +1735,2209 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:23" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:23" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>45730.601728773152</v>
       </c>
       <c r="B2" s="5" t="s">
+        <v>252</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="D2" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="E2" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="F2" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="G2" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="H2" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="I2" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="J2" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="K2" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="K2" s="5" t="s">
+      <c r="L2" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="L2" s="5" t="s">
-        <v>33</v>
-      </c>
       <c r="M2" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="N2" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="N2" s="5" t="s">
+      <c r="O2" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="P2" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="O2" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="P2" s="5" t="s">
+      <c r="Q2" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="Q2" s="5" t="s">
+      <c r="R2" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="R2" s="5" t="s">
+      <c r="S2" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="S2" s="5" t="s">
+      <c r="T2" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="T2" s="5" t="s">
+      <c r="U2" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="U2" s="5" t="s">
+      <c r="V2" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="V2" s="5" t="s">
+      <c r="W2" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="W2" s="6" t="s">
-        <v>43</v>
-      </c>
     </row>
-    <row r="3" spans="1:23" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:23" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A3" s="7">
         <v>45743.586425486108</v>
       </c>
       <c r="B3" s="8" t="s">
+        <v>253</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="F3" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="D3" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="E3" s="8" t="s">
+      <c r="G3" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="H3" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="I3" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="G3" s="8" t="s">
+      <c r="J3" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="H3" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="I3" s="8" t="s">
+      <c r="K3" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="L3" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="M3" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="N3" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="J3" s="8" t="s">
+      <c r="O3" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="P3" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="K3" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="L3" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="M3" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="N3" s="8" t="s">
+      <c r="Q3" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="O3" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="P3" s="8" t="s">
+      <c r="R3" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="Q3" s="8" t="s">
+      <c r="S3" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="R3" s="8" t="s">
+      <c r="T3" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="S3" s="8" t="s">
+      <c r="U3" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="T3" s="8" t="s">
+      <c r="V3" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="U3" s="8" t="s">
+      <c r="W3" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="V3" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="W3" s="9" t="s">
-        <v>59</v>
-      </c>
     </row>
-    <row r="4" spans="1:23" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:23" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>45719.731454016204</v>
       </c>
       <c r="B4" s="5" t="s">
+        <v>256</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="F4" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="G4" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="J4" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="D4" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="E4" s="5" t="s">
+      <c r="K4" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="L4" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="M4" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="N4" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="G4" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="H4" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="I4" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="J4" s="5" t="s">
+      <c r="O4" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="K4" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="L4" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="M4" s="5" t="s">
+      <c r="P4" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="N4" s="5" t="s">
+      <c r="Q4" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="O4" s="5" t="s">
+      <c r="R4" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="P4" s="5" t="s">
+      <c r="S4" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="Q4" s="5" t="s">
+      <c r="T4" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="R4" s="5" t="s">
+      <c r="U4" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="S4" s="5" t="s">
+      <c r="V4" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="T4" s="5" t="s">
+      <c r="W4" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="U4" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="V4" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="W4" s="6" t="s">
-        <v>75</v>
-      </c>
     </row>
-    <row r="5" spans="1:23" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:23" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A5" s="7">
         <v>45730.57488482639</v>
       </c>
       <c r="B5" s="8" t="s">
+        <v>257</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="H5" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="I5" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="J5" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="K5" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="L5" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="M5" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="N5" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="O5" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="D5" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="E5" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="F5" s="8" t="s">
+      <c r="P5" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="G5" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="H5" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="I5" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="J5" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="K5" s="8" t="s">
+      <c r="Q5" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="L5" s="8" t="s">
+      <c r="R5" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="M5" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="N5" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="O5" s="8" t="s">
+      <c r="S5" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="P5" s="8" t="s">
+      <c r="T5" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="U5" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="Q5" s="8" t="s">
+      <c r="V5" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="R5" s="8" t="s">
+      <c r="W5" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="S5" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="T5" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="U5" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="V5" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="W5" s="9" t="s">
-        <v>88</v>
-      </c>
     </row>
-    <row r="6" spans="1:23" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:23" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>45730.584843958335</v>
       </c>
       <c r="B6" s="5" t="s">
+        <v>258</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="J6" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="K6" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="L6" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="M6" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="N6" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="O6" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="P6" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="Q6" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="R6" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="C6" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="D6" s="5" t="s">
+      <c r="S6" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="E6" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="G6" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="H6" s="5" t="s">
+      <c r="T6" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="U6" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="V6" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="I6" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="J6" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="K6" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="L6" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="M6" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="N6" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="O6" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="P6" s="5" t="s">
+      <c r="W6" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="Q6" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="R6" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="S6" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="T6" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="U6" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="V6" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="W6" s="6" t="s">
-        <v>97</v>
-      </c>
     </row>
-    <row r="7" spans="1:23" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:23" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A7" s="7">
         <v>45715.844303854166</v>
       </c>
       <c r="B7" s="8" t="s">
+        <v>255</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="H7" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="I7" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="J7" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="K7" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="L7" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="M7" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="N7" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="O7" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="P7" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="Q7" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="R7" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="S7" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="C7" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="E7" s="8" t="s">
+      <c r="T7" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="U7" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="F7" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="G7" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="H7" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="I7" s="8" t="s">
+      <c r="V7" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="J7" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="K7" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="L7" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="M7" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="N7" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="O7" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="P7" s="8" t="s">
+      <c r="W7" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="Q7" s="8" t="s">
-        <v>102</v>
-      </c>
-      <c r="R7" s="8" t="s">
-        <v>103</v>
-      </c>
-      <c r="S7" s="8" t="s">
-        <v>104</v>
-      </c>
-      <c r="T7" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="U7" s="8" t="s">
-        <v>105</v>
-      </c>
-      <c r="V7" s="8" t="s">
-        <v>106</v>
-      </c>
-      <c r="W7" s="9" t="s">
-        <v>107</v>
-      </c>
     </row>
-    <row r="8" spans="1:23" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:23" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>45734.464259409724</v>
       </c>
       <c r="B8" s="5" t="s">
+        <v>259</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="I8" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="J8" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="K8" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="L8" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="M8" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="N8" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="O8" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="P8" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="Q8" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="R8" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="C8" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="D8" s="5" t="s">
+      <c r="S8" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="T8" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="U8" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="V8" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="F8" s="5" t="s">
+      <c r="W8" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="G8" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="H8" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="I8" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="J8" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="K8" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="L8" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="M8" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="N8" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="O8" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="P8" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="Q8" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="R8" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="S8" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="T8" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="U8" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="V8" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="W8" s="6" t="s">
-        <v>118</v>
-      </c>
     </row>
-    <row r="9" spans="1:23" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:23" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A9" s="7">
         <v>45722.649656261579</v>
       </c>
       <c r="B9" s="8" t="s">
+        <v>254</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="H9" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="I9" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="J9" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="K9" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="L9" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="M9" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="N9" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="O9" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="P9" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="Q9" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="R9" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="S9" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="T9" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="U9" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="V9" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="W9" s="9" t="s">
         <v>119</v>
       </c>
-      <c r="C9" s="8" t="s">
-        <v>120</v>
-      </c>
-      <c r="D9" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="E9" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="F9" s="8" t="s">
-        <v>111</v>
-      </c>
-      <c r="G9" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="H9" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="I9" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="J9" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="K9" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="L9" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="M9" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="N9" s="8" t="s">
-        <v>121</v>
-      </c>
-      <c r="O9" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="P9" s="8" t="s">
-        <v>122</v>
-      </c>
-      <c r="Q9" s="8" t="s">
-        <v>123</v>
-      </c>
-      <c r="R9" s="8" t="s">
-        <v>124</v>
-      </c>
-      <c r="S9" s="8" t="s">
-        <v>125</v>
-      </c>
-      <c r="T9" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="U9" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="V9" s="8" t="s">
-        <v>126</v>
-      </c>
-      <c r="W9" s="9" t="s">
-        <v>127</v>
-      </c>
     </row>
-    <row r="10" spans="1:23" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:23" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>45737.388240636574</v>
       </c>
       <c r="B10" s="5" t="s">
+        <v>260</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="H10" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="I10" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="J10" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="K10" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="L10" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="M10" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="N10" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="O10" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="P10" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q10" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="R10" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="S10" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="T10" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="U10" s="5" t="s">
         <v>128</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="V10" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="W10" s="6" t="s">
         <v>130</v>
       </c>
-      <c r="E10" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="G10" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="H10" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="I10" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="J10" s="5" t="s">
-        <v>132</v>
-      </c>
-      <c r="K10" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="L10" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="M10" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="N10" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="O10" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="P10" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="Q10" s="5" t="s">
-        <v>134</v>
-      </c>
-      <c r="R10" s="5" t="s">
-        <v>135</v>
-      </c>
-      <c r="S10" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="T10" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="U10" s="5" t="s">
-        <v>137</v>
-      </c>
-      <c r="V10" s="5" t="s">
-        <v>138</v>
-      </c>
-      <c r="W10" s="6" t="s">
-        <v>139</v>
-      </c>
     </row>
-    <row r="11" spans="1:23" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:23" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A11" s="7">
         <v>45718.535542164347</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>140</v>
+        <v>261</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
       <c r="G11" s="8" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="H11" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I11" s="8" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="J11" s="8" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="K11" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="L11" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="L11" s="8" t="s">
-        <v>33</v>
-      </c>
       <c r="M11" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="N11" s="8" t="s">
         <v>113</v>
       </c>
-      <c r="N11" s="8" t="s">
-        <v>121</v>
-      </c>
       <c r="O11" s="8" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="P11" s="8" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
       <c r="Q11" s="8" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="R11" s="8" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="S11" s="8" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="T11" s="8" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="U11" s="8" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="V11" s="8" t="s">
-        <v>145</v>
+        <v>135</v>
       </c>
       <c r="W11" s="9" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
     </row>
-    <row r="12" spans="1:23" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:23" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>45722.902199062504</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>147</v>
+        <v>262</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>148</v>
+        <v>137</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>149</v>
+        <v>138</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="H12" s="5" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="I12" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J12" s="5" t="s">
-        <v>150</v>
+        <v>139</v>
       </c>
       <c r="K12" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="L12" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="L12" s="5" t="s">
-        <v>33</v>
-      </c>
       <c r="M12" s="5" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="N12" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="O12" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="P12" s="5" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="Q12" s="5" t="s">
-        <v>151</v>
+        <v>140</v>
       </c>
       <c r="R12" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="S12" s="5" t="s">
-        <v>152</v>
+        <v>141</v>
       </c>
       <c r="T12" s="5" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="U12" s="5" t="s">
-        <v>153</v>
+        <v>142</v>
       </c>
       <c r="V12" s="5" t="s">
-        <v>154</v>
+        <v>143</v>
       </c>
       <c r="W12" s="6" t="s">
-        <v>155</v>
+        <v>144</v>
       </c>
     </row>
-    <row r="13" spans="1:23" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:23" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A13" s="7">
         <v>45744.803429039355</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>156</v>
+        <v>263</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="E13" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="G13" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="H13" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="I13" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="J13" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="K13" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="L13" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="M13" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="N13" s="8" t="s">
         <v>148</v>
       </c>
-      <c r="F13" s="8" t="s">
-        <v>158</v>
-      </c>
-      <c r="G13" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="H13" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="I13" s="8" t="s">
-        <v>159</v>
-      </c>
-      <c r="J13" s="8" t="s">
-        <v>132</v>
-      </c>
-      <c r="K13" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="L13" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="M13" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="N13" s="8" t="s">
-        <v>160</v>
-      </c>
       <c r="O13" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="P13" s="8" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
       <c r="Q13" s="8" t="s">
-        <v>162</v>
+        <v>150</v>
       </c>
       <c r="R13" s="8" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="S13" s="8" t="s">
-        <v>163</v>
+        <v>151</v>
       </c>
       <c r="T13" s="8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="U13" s="8" t="s">
-        <v>164</v>
+        <v>152</v>
       </c>
       <c r="V13" s="8" t="s">
-        <v>165</v>
+        <v>153</v>
       </c>
       <c r="W13" s="9" t="s">
-        <v>166</v>
+        <v>154</v>
       </c>
     </row>
-    <row r="14" spans="1:23" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:23" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
         <v>45722.708462199073</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>167</v>
+        <v>264</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>168</v>
+        <v>155</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>169</v>
+        <v>156</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="H14" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I14" s="5" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="J14" s="5" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="K14" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="L14" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="L14" s="5" t="s">
-        <v>33</v>
-      </c>
       <c r="M14" s="5" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="N14" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="O14" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="P14" s="5" t="s">
-        <v>170</v>
+        <v>157</v>
       </c>
       <c r="Q14" s="5" t="s">
-        <v>171</v>
+        <v>158</v>
       </c>
       <c r="R14" s="5" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="S14" s="5" t="s">
-        <v>172</v>
+        <v>159</v>
       </c>
       <c r="T14" s="5" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="U14" s="5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="V14" s="5" t="s">
-        <v>173</v>
+        <v>160</v>
       </c>
       <c r="W14" s="6" t="s">
-        <v>174</v>
+        <v>161</v>
       </c>
     </row>
-    <row r="15" spans="1:23" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:23" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A15" s="7">
         <v>45715.739319756947</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>175</v>
+        <v>265</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>176</v>
+        <v>162</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F15" s="8" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="G15" s="8" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="H15" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I15" s="8" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="J15" s="8" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="K15" s="8" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="L15" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="M15" s="8" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="N15" s="8" t="s">
-        <v>160</v>
+        <v>148</v>
       </c>
       <c r="O15" s="8" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="P15" s="8" t="s">
-        <v>177</v>
+        <v>163</v>
       </c>
       <c r="Q15" s="8" t="s">
-        <v>178</v>
+        <v>164</v>
       </c>
       <c r="R15" s="8" t="s">
-        <v>179</v>
+        <v>165</v>
       </c>
       <c r="S15" s="8" t="s">
-        <v>180</v>
+        <v>166</v>
       </c>
       <c r="T15" s="8" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="U15" s="8" t="s">
-        <v>181</v>
+        <v>167</v>
       </c>
       <c r="V15" s="8" t="s">
-        <v>182</v>
+        <v>168</v>
       </c>
       <c r="W15" s="9" t="s">
-        <v>183</v>
+        <v>169</v>
       </c>
     </row>
-    <row r="16" spans="1:23" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:23" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
         <v>45743.784772141204</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>184</v>
+        <v>266</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>185</v>
+        <v>170</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>186</v>
+        <v>171</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>149</v>
+        <v>138</v>
       </c>
       <c r="G16" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="H16" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="H16" s="5" t="s">
-        <v>29</v>
-      </c>
       <c r="I16" s="5" t="s">
-        <v>187</v>
+        <v>172</v>
       </c>
       <c r="J16" s="5" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="K16" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="L16" s="5" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="M16" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="N16" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="N16" s="5" t="s">
-        <v>121</v>
-      </c>
       <c r="O16" s="5" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="P16" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="Q16" s="5" t="s">
-        <v>188</v>
+        <v>173</v>
       </c>
       <c r="R16" s="5" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="S16" s="5" t="s">
-        <v>189</v>
+        <v>174</v>
       </c>
       <c r="T16" s="5" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="U16" s="5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="V16" s="5" t="s">
-        <v>190</v>
+        <v>175</v>
       </c>
       <c r="W16" s="6" t="s">
-        <v>191</v>
+        <v>176</v>
       </c>
     </row>
-    <row r="17" spans="1:23" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:23" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A17" s="7">
         <v>45730.773973009258</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>192</v>
+        <v>267</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>186</v>
+        <v>171</v>
       </c>
       <c r="F17" s="8" t="s">
-        <v>193</v>
+        <v>177</v>
       </c>
       <c r="G17" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="H17" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="H17" s="8" t="s">
+      <c r="I17" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="I17" s="8" t="s">
-        <v>30</v>
-      </c>
       <c r="J17" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="K17" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="L17" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="M17" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="N17" s="8" t="s">
+        <v>178</v>
+      </c>
+      <c r="O17" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="P17" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="K17" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="L17" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="M17" s="8" t="s">
-        <v>113</v>
-      </c>
-      <c r="N17" s="8" t="s">
-        <v>194</v>
-      </c>
-      <c r="O17" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="P17" s="8" t="s">
-        <v>52</v>
-      </c>
       <c r="Q17" s="8" t="s">
-        <v>195</v>
+        <v>179</v>
       </c>
       <c r="R17" s="8" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="S17" s="8" t="s">
-        <v>196</v>
+        <v>180</v>
       </c>
       <c r="T17" s="8" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="U17" s="8" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="V17" s="8" t="s">
-        <v>197</v>
+        <v>181</v>
       </c>
       <c r="W17" s="9" t="s">
-        <v>198</v>
+        <v>182</v>
       </c>
     </row>
-    <row r="18" spans="1:23" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:23" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
         <v>45723.61265314815</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>199</v>
+        <v>268</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>200</v>
+        <v>183</v>
       </c>
       <c r="D18" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E18" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E18" s="5" t="s">
-        <v>26</v>
-      </c>
       <c r="F18" s="5" t="s">
-        <v>201</v>
+        <v>184</v>
       </c>
       <c r="G18" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="H18" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="H18" s="5" t="s">
+      <c r="I18" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="I18" s="5" t="s">
-        <v>30</v>
-      </c>
       <c r="J18" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="K18" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="L18" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="M18" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="N18" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="O18" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="K18" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="L18" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="M18" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="N18" s="5" t="s">
-        <v>160</v>
-      </c>
-      <c r="O18" s="5" t="s">
+      <c r="P18" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="Q18" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="R18" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="P18" s="5" t="s">
-        <v>161</v>
-      </c>
-      <c r="Q18" s="5" t="s">
-        <v>202</v>
-      </c>
-      <c r="R18" s="5" t="s">
-        <v>70</v>
-      </c>
       <c r="S18" s="5" t="s">
-        <v>203</v>
+        <v>186</v>
       </c>
       <c r="T18" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="U18" s="5" t="s">
-        <v>164</v>
+        <v>152</v>
       </c>
       <c r="V18" s="5" t="s">
-        <v>204</v>
+        <v>187</v>
       </c>
       <c r="W18" s="6" t="s">
-        <v>205</v>
+        <v>188</v>
       </c>
     </row>
-    <row r="19" spans="1:23" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:23" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A19" s="7">
         <v>45716.618010694445</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>206</v>
+        <v>269</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>207</v>
+        <v>189</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E19" s="8" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F19" s="8" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
       <c r="G19" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="H19" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="H19" s="8" t="s">
-        <v>29</v>
-      </c>
       <c r="I19" s="8" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="J19" s="8" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="K19" s="8" t="s">
-        <v>208</v>
+        <v>190</v>
       </c>
       <c r="L19" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="M19" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="N19" s="8" t="s">
         <v>113</v>
       </c>
-      <c r="N19" s="8" t="s">
-        <v>121</v>
-      </c>
       <c r="O19" s="8" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="P19" s="8" t="s">
-        <v>209</v>
+        <v>191</v>
       </c>
       <c r="Q19" s="8" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="R19" s="8" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="S19" s="8" t="s">
-        <v>210</v>
+        <v>192</v>
       </c>
       <c r="T19" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="U19" s="8" t="s">
-        <v>211</v>
+        <v>193</v>
       </c>
       <c r="V19" s="8" t="s">
-        <v>212</v>
+        <v>194</v>
       </c>
       <c r="W19" s="9" t="s">
-        <v>213</v>
+        <v>195</v>
       </c>
     </row>
-    <row r="20" spans="1:23" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:23" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
         <v>45722.55565415509</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>214</v>
+        <v>270</v>
       </c>
       <c r="C20" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D20" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="D20" s="5" t="s">
-        <v>25</v>
-      </c>
       <c r="E20" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="G20" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="F20" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="G20" s="5" t="s">
+      <c r="H20" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="I20" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="J20" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="H20" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="I20" s="5" t="s">
-        <v>215</v>
-      </c>
-      <c r="J20" s="5" t="s">
-        <v>50</v>
-      </c>
       <c r="K20" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="L20" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="M20" s="5" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="N20" s="5" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="O20" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="P20" s="5" t="s">
-        <v>216</v>
+        <v>197</v>
       </c>
       <c r="Q20" s="5" t="s">
-        <v>217</v>
+        <v>198</v>
       </c>
       <c r="R20" s="5" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="S20" s="5" t="s">
-        <v>218</v>
+        <v>199</v>
       </c>
       <c r="T20" s="5" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="U20" s="5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="V20" s="5" t="s">
-        <v>216</v>
+        <v>197</v>
       </c>
       <c r="W20" s="6" t="s">
-        <v>216</v>
+        <v>197</v>
       </c>
     </row>
-    <row r="21" spans="1:23" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:23" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A21" s="7">
         <v>45728.904280162038</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>219</v>
+        <v>271</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>220</v>
+        <v>200</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>221</v>
+        <v>201</v>
       </c>
       <c r="F21" s="8" t="s">
-        <v>158</v>
+        <v>146</v>
       </c>
       <c r="G21" s="8" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="H21" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="I21" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="I21" s="8" t="s">
-        <v>30</v>
-      </c>
       <c r="J21" s="8" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="K21" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="L21" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="L21" s="8" t="s">
-        <v>33</v>
-      </c>
       <c r="M21" s="8" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="N21" s="8" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="O21" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="P21" s="8" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
       <c r="Q21" s="8" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="R21" s="8" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="S21" s="8" t="s">
-        <v>222</v>
+        <v>202</v>
       </c>
       <c r="T21" s="8" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="U21" s="8" t="s">
-        <v>223</v>
+        <v>203</v>
       </c>
       <c r="V21" s="8" t="s">
-        <v>224</v>
+        <v>204</v>
       </c>
       <c r="W21" s="9" t="s">
-        <v>225</v>
+        <v>205</v>
       </c>
     </row>
-    <row r="22" spans="1:23" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:23" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
         <v>45743.742979768518</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>226</v>
+        <v>272</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>227</v>
+        <v>206</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="G22" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="H22" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="H22" s="5" t="s">
-        <v>29</v>
-      </c>
       <c r="I22" s="5" t="s">
-        <v>215</v>
+        <v>196</v>
       </c>
       <c r="J22" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K22" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="L22" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="M22" s="5" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="N22" s="5" t="s">
-        <v>160</v>
+        <v>148</v>
       </c>
       <c r="O22" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="P22" s="5" t="s">
-        <v>228</v>
+        <v>207</v>
       </c>
       <c r="Q22" s="5" t="s">
-        <v>229</v>
+        <v>208</v>
       </c>
       <c r="R22" s="5" t="s">
-        <v>230</v>
+        <v>209</v>
       </c>
       <c r="S22" s="5" t="s">
-        <v>231</v>
+        <v>210</v>
       </c>
       <c r="T22" s="5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="U22" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="V22" s="5" t="s">
         <v>211</v>
       </c>
-      <c r="V22" s="5" t="s">
-        <v>232</v>
-      </c>
       <c r="W22" s="6" t="s">
-        <v>233</v>
+        <v>212</v>
       </c>
     </row>
-    <row r="23" spans="1:23" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:23" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A23" s="7">
         <v>45717.79771648148</v>
       </c>
-      <c r="B23" s="8"/>
+      <c r="B23" s="8" t="s">
+        <v>273</v>
+      </c>
       <c r="C23" s="8" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="E23" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F23" s="8" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="G23" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="H23" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="I23" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="J23" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="H23" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="I23" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="J23" s="8" t="s">
-        <v>50</v>
-      </c>
       <c r="K23" s="8" t="s">
-        <v>208</v>
+        <v>190</v>
       </c>
       <c r="L23" s="8" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="M23" s="8" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="N23" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="O23" s="8" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="P23" s="8" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="Q23" s="8" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="R23" s="8" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="S23" s="8" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="T23" s="8" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="U23" s="8" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="V23" s="8" t="s">
-        <v>234</v>
+        <v>213</v>
       </c>
       <c r="W23" s="9" t="s">
-        <v>235</v>
+        <v>214</v>
       </c>
     </row>
-    <row r="24" spans="1:23" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:23" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A24" s="4">
         <v>45724.504372453703</v>
       </c>
-      <c r="B24" s="5"/>
+      <c r="B24" s="5" t="s">
+        <v>274</v>
+      </c>
       <c r="C24" s="5" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>236</v>
+        <v>215</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="G24" s="5" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="H24" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I24" s="5" t="s">
-        <v>237</v>
+        <v>216</v>
       </c>
       <c r="J24" s="5" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="K24" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L24" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="M24" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="N24" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="M24" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="N24" s="5" t="s">
-        <v>35</v>
-      </c>
       <c r="O24" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="P24" s="5" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="Q24" s="5" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="R24" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="S24" s="5" t="s">
-        <v>238</v>
+        <v>217</v>
       </c>
       <c r="T24" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="U24" s="5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="V24" s="5" t="s">
-        <v>239</v>
+        <v>218</v>
       </c>
       <c r="W24" s="6" t="s">
-        <v>240</v>
+        <v>219</v>
       </c>
     </row>
-    <row r="25" spans="1:23" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:23" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A25" s="7">
         <v>45715.749944895833</v>
       </c>
-      <c r="B25" s="8"/>
+      <c r="B25" s="8" t="s">
+        <v>275</v>
+      </c>
       <c r="C25" s="8" t="s">
-        <v>176</v>
+        <v>162</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E25" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="F25" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="G25" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="F25" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="G25" s="8" t="s">
-        <v>48</v>
-      </c>
       <c r="H25" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I25" s="8" t="s">
-        <v>215</v>
+        <v>196</v>
       </c>
       <c r="J25" s="8" t="s">
-        <v>150</v>
+        <v>139</v>
       </c>
       <c r="K25" s="8" t="s">
-        <v>208</v>
+        <v>190</v>
       </c>
       <c r="L25" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="M25" s="8" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="N25" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="O25" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="P25" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="O25" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="P25" s="8" t="s">
-        <v>36</v>
-      </c>
       <c r="Q25" s="8" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="R25" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="S25" s="8" t="s">
-        <v>163</v>
+        <v>151</v>
       </c>
       <c r="T25" s="8" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="U25" s="8" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="V25" s="8" t="s">
-        <v>241</v>
+        <v>220</v>
       </c>
       <c r="W25" s="9" t="s">
-        <v>242</v>
+        <v>221</v>
       </c>
     </row>
-    <row r="26" spans="1:23" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:23" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A26" s="4">
         <v>45730.618392372686</v>
       </c>
-      <c r="B26" s="5"/>
+      <c r="B26" s="5" t="s">
+        <v>276</v>
+      </c>
       <c r="C26" s="5" t="s">
-        <v>168</v>
+        <v>155</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E26" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="F26" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="G26" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="F26" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="G26" s="5" t="s">
-        <v>48</v>
-      </c>
       <c r="H26" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="I26" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="I26" s="5" t="s">
-        <v>30</v>
-      </c>
       <c r="J26" s="5" t="s">
-        <v>150</v>
+        <v>139</v>
       </c>
       <c r="K26" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="L26" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="L26" s="5" t="s">
-        <v>33</v>
-      </c>
       <c r="M26" s="5" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="N26" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="O26" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="P26" s="5" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="Q26" s="5" t="s">
-        <v>243</v>
+        <v>222</v>
       </c>
       <c r="R26" s="5" t="s">
-        <v>244</v>
+        <v>223</v>
       </c>
       <c r="S26" s="5" t="s">
-        <v>245</v>
+        <v>224</v>
       </c>
       <c r="T26" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="U26" s="5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="V26" s="5" t="s">
-        <v>246</v>
+        <v>225</v>
       </c>
       <c r="W26" s="6" t="s">
-        <v>247</v>
+        <v>226</v>
       </c>
     </row>
-    <row r="27" spans="1:23" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:23" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A27" s="7">
         <v>45741.380899282405</v>
       </c>
+      <c r="B27" s="8" t="s">
+        <v>277</v>
+      </c>
       <c r="C27" s="8" t="s">
-        <v>220</v>
+        <v>200</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="E27" s="8" t="s">
+        <v>206</v>
+      </c>
+      <c r="F27" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="G27" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="H27" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="I27" s="8" t="s">
         <v>227</v>
       </c>
-      <c r="F27" s="8" t="s">
-        <v>141</v>
-      </c>
-      <c r="G27" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="H27" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="I27" s="8" t="s">
-        <v>248</v>
-      </c>
       <c r="J27" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="K27" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="K27" s="8" t="s">
+      <c r="L27" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="L27" s="8" t="s">
-        <v>33</v>
-      </c>
       <c r="M27" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="N27" s="8" t="s">
         <v>113</v>
       </c>
-      <c r="N27" s="8" t="s">
-        <v>121</v>
-      </c>
       <c r="O27" s="8" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="P27" s="8" t="s">
-        <v>249</v>
+        <v>228</v>
       </c>
       <c r="Q27" s="8" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="R27" s="8" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="S27" s="8" t="s">
-        <v>250</v>
+        <v>229</v>
       </c>
       <c r="T27" s="8" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="U27" s="8" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="V27" s="8" t="s">
-        <v>251</v>
+        <v>230</v>
       </c>
       <c r="W27" s="9" t="s">
-        <v>252</v>
+        <v>231</v>
       </c>
     </row>
-    <row r="28" spans="1:23" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:23" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A28" s="4">
         <v>45736.863093055552</v>
       </c>
+      <c r="B28" s="5" t="s">
+        <v>278</v>
+      </c>
       <c r="C28" s="5" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>186</v>
+        <v>171</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="G28" s="5" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="H28" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I28" s="5" t="s">
-        <v>253</v>
+        <v>232</v>
       </c>
       <c r="J28" s="5" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="K28" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="L28" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="L28" s="5" t="s">
-        <v>33</v>
-      </c>
       <c r="M28" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="N28" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="N28" s="5" t="s">
-        <v>121</v>
-      </c>
       <c r="O28" s="5" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="P28" s="5" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="Q28" s="5" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="R28" s="5" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="S28" s="5" t="s">
-        <v>254</v>
+        <v>233</v>
       </c>
       <c r="T28" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="U28" s="5" t="s">
-        <v>164</v>
+        <v>152</v>
       </c>
       <c r="V28" s="5" t="s">
-        <v>255</v>
+        <v>234</v>
       </c>
       <c r="W28" s="6" t="s">
-        <v>256</v>
+        <v>235</v>
       </c>
     </row>
-    <row r="29" spans="1:23" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:23" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A29" s="7">
         <v>45722.918789814816</v>
       </c>
-      <c r="B29" s="8"/>
+      <c r="B29" s="8" t="s">
+        <v>279</v>
+      </c>
       <c r="C29" s="8" t="s">
-        <v>257</v>
+        <v>236</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E29" s="8" t="s">
-        <v>186</v>
+        <v>171</v>
       </c>
       <c r="F29" s="8" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="G29" s="8" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="H29" s="8" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="I29" s="8" t="s">
-        <v>258</v>
+        <v>237</v>
       </c>
       <c r="J29" s="8" t="s">
-        <v>150</v>
+        <v>139</v>
       </c>
       <c r="K29" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L29" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="M29" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="N29" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="O29" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="P29" s="8" t="s">
         <v>133</v>
       </c>
-      <c r="M29" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="N29" s="8" t="s">
-        <v>121</v>
-      </c>
-      <c r="O29" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="P29" s="8" t="s">
-        <v>143</v>
-      </c>
       <c r="Q29" s="8" t="s">
-        <v>259</v>
+        <v>238</v>
       </c>
       <c r="R29" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="S29" s="8" t="s">
-        <v>260</v>
+        <v>239</v>
       </c>
       <c r="T29" s="8" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="U29" s="8" t="s">
-        <v>223</v>
+        <v>203</v>
       </c>
       <c r="V29" s="8" t="s">
-        <v>261</v>
+        <v>240</v>
       </c>
       <c r="W29" s="9" t="s">
-        <v>262</v>
+        <v>241</v>
       </c>
     </row>
-    <row r="30" spans="1:23" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:23" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="4">
         <v>45724.369019849539</v>
       </c>
-      <c r="B30" s="5"/>
+      <c r="B30" s="5" t="s">
+        <v>280</v>
+      </c>
       <c r="C30" s="5" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>227</v>
+        <v>206</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G30" s="5" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="H30" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="I30" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="I30" s="5" t="s">
-        <v>30</v>
-      </c>
       <c r="J30" s="5" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="K30" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="L30" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="M30" s="5" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="N30" s="5" t="s">
-        <v>160</v>
+        <v>148</v>
       </c>
       <c r="O30" s="5" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="P30" s="5" t="s">
-        <v>228</v>
+        <v>207</v>
       </c>
       <c r="Q30" s="5" t="s">
-        <v>263</v>
+        <v>242</v>
       </c>
       <c r="R30" s="5" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="S30" s="5" t="s">
-        <v>264</v>
+        <v>243</v>
       </c>
       <c r="T30" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="U30" s="5" t="s">
-        <v>211</v>
+        <v>193</v>
       </c>
       <c r="V30" s="5" t="s">
-        <v>265</v>
+        <v>244</v>
       </c>
       <c r="W30" s="6" t="s">
-        <v>265</v>
+        <v>244</v>
       </c>
     </row>
-    <row r="31" spans="1:23" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:23" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A31" s="7">
         <v>45725.761683657409</v>
       </c>
-      <c r="B31" s="8"/>
+      <c r="B31" s="8" t="s">
+        <v>281</v>
+      </c>
       <c r="C31" s="8" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="E31" s="8" t="s">
-        <v>148</v>
+        <v>137</v>
       </c>
       <c r="F31" s="8" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
       <c r="G31" s="8" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="H31" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="I31" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="I31" s="8" t="s">
-        <v>30</v>
-      </c>
       <c r="J31" s="8" t="s">
-        <v>150</v>
+        <v>139</v>
       </c>
       <c r="K31" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="L31" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="M31" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="N31" s="8" t="s">
-        <v>266</v>
+        <v>245</v>
       </c>
       <c r="O31" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="P31" s="8" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="Q31" s="8" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="R31" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="S31" s="8" t="s">
+        <v>246</v>
+      </c>
+      <c r="T31" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="S31" s="8" t="s">
-        <v>267</v>
-      </c>
-      <c r="T31" s="8" t="s">
-        <v>56</v>
-      </c>
       <c r="U31" s="8" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="V31" s="8" t="s">
-        <v>268</v>
+        <v>247</v>
       </c>
       <c r="W31" s="9" t="s">
-        <v>166</v>
+        <v>154</v>
       </c>
     </row>
-    <row r="32" spans="1:23" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:23" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A32" s="10">
         <v>45741.741304907409</v>
       </c>
+      <c r="B32" s="5" t="s">
+        <v>282</v>
+      </c>
       <c r="C32" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="D32" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="E32" s="11" t="s">
+        <v>171</v>
+      </c>
+      <c r="F32" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="G32" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="H32" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="I32" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="J32" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="D32" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="E32" s="11" t="s">
-        <v>186</v>
-      </c>
-      <c r="F32" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="G32" s="11" t="s">
-        <v>112</v>
-      </c>
-      <c r="H32" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="I32" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="J32" s="11" t="s">
-        <v>64</v>
-      </c>
       <c r="K32" s="11" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="L32" s="11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="M32" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="N32" s="11" t="s">
+        <v>148</v>
+      </c>
+      <c r="O32" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="P32" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="N32" s="11" t="s">
-        <v>160</v>
-      </c>
-      <c r="O32" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="P32" s="11" t="s">
-        <v>68</v>
-      </c>
       <c r="Q32" s="11" t="s">
-        <v>269</v>
+        <v>248</v>
       </c>
       <c r="R32" s="11" t="s">
-        <v>179</v>
+        <v>165</v>
       </c>
       <c r="S32" s="11" t="s">
-        <v>270</v>
+        <v>249</v>
       </c>
       <c r="T32" s="11" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="U32" s="11" t="s">
-        <v>211</v>
+        <v>193</v>
       </c>
       <c r="V32" s="11" t="s">
-        <v>271</v>
+        <v>250</v>
       </c>
       <c r="W32" s="12" t="s">
-        <v>272</v>
+        <v>251</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>

</xml_diff>